<commit_message>
external volume and cron backup for db
</commit_message>
<xml_diff>
--- a/ADMIN_ExcelFile.xlsx
+++ b/ADMIN_ExcelFile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="57" count="57">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="64" count="64">
   <x:si>
     <x:t>_id</x:t>
   </x:si>
@@ -58,7 +58,7 @@
     <x:t>latest_dose_date</x:t>
   </x:si>
   <x:si>
-    <x:t>612b6e972fd1e10044822f37</x:t>
+    <x:t>612c446e21b1190043d71b5d</x:t>
   </x:si>
   <x:si>
     <x:t>https://lh3.googleusercontent.com/a-/AOh14Gj1ww5UEswYptQPWEoVEaPYRkThY6c5A9AJQmVd=s96-c</x:t>
@@ -85,106 +85,127 @@
     <x:t>media/consent/f20200048@pilani.bits-pilani.ac.in.pdf</x:t>
   </x:si>
   <x:si>
+    <x:t>Tue Sep 21 2021 04:30:00 GMT+0000 (Coordinated Universal Time)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>612c44dc82a6e7f8ae653cf4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MOHIT 2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>f20200047@pilani.bits-pilani.ac.in</x:t>
+  </x:si>
+  <x:si>
     <x:t>Tue Sep 21 2021 16:30:00 GMT+0000 (Coordinated Universal Time)</x:t>
   </x:si>
   <x:si>
-    <x:t>612b7278fdaa04d6486cb7e2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MOHIT MAKWANA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>f20190049@pilani.bits-pilani.ac.in</x:t>
+    <x:t>612c44f082a6e7f8ae653cf6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MOHIT 3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>f20190047@pilani.bits-pilani.ac.in</x:t>
   </x:si>
   <x:si>
     <x:t>Tue Sep 21 2021 16:30:00 GMT+0000 (Coordinated Universal Time)</x:t>
   </x:si>
   <x:si>
-    <x:t>612b7292fdaa04d6486cb7e4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>f20200047@pilani.bits-pilani.ac.in</x:t>
+    <x:t>612c450282a6e7f8ae653cf8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MOHIT 4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>f20180047@pilani.bits-pilani.ac.in</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Thu Jan 21 2021 16:30:00 GMT+0000 (Coordinated Universal Time)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>612c451c82a6e7f8ae653cfa</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MOHIT 5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>f20190000@pilani.bits-pilani.ac.in</x:t>
   </x:si>
   <x:si>
     <x:t>Tue Sep 21 2021 16:30:00 GMT+0000 (Coordinated Universal Time)</x:t>
   </x:si>
   <x:si>
-    <x:t>612b72b1fdaa04d6486cb7e6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>f20190046@pilani.bits-pilani.ac.in</x:t>
+    <x:t>612c453082a6e7f8ae653cfc</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MOHIT 6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>f20180027@pilani.bits-pilani.ac.in</x:t>
   </x:si>
   <x:si>
     <x:t>Tue Sep 21 2021 16:30:00 GMT+0000 (Coordinated Universal Time)</x:t>
   </x:si>
   <x:si>
-    <x:t>612b72ccfdaa04d6486cb7e8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>f20200045@pilani.bits-pilani.ac.in</x:t>
+    <x:t>612c454782a6e7f8ae653cfe</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MOHIT 7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>f20200037@pilani.bits-pilani.ac.in</x:t>
   </x:si>
   <x:si>
     <x:t>Tue Sep 21 2021 16:30:00 GMT+0000 (Coordinated Universal Time)</x:t>
   </x:si>
   <x:si>
-    <x:t>612b72d6fdaa04d6486cb7ea</x:t>
-  </x:si>
-  <x:si>
-    <x:t>f20180044@pilani.bits-pilani.ac.in</x:t>
+    <x:t>612c455582a6e7f8ae653d00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MOHIT 8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>f20200041@pilani.bits-pilani.ac.in</x:t>
   </x:si>
   <x:si>
     <x:t>Tue Sep 21 2021 16:30:00 GMT+0000 (Coordinated Universal Time)</x:t>
   </x:si>
   <x:si>
-    <x:t>612b72e0fdaa04d6486cb7ec</x:t>
-  </x:si>
-  <x:si>
-    <x:t>f20200043@pilani.bits-pilani.ac.in</x:t>
+    <x:t>612c456882a6e7f8ae653d02</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MOHIT 9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>f20190042@pilani.bits-pilani.ac.in</x:t>
   </x:si>
   <x:si>
     <x:t>Tue Sep 21 2021 16:30:00 GMT+0000 (Coordinated Universal Time)</x:t>
   </x:si>
   <x:si>
-    <x:t>612b72e8fdaa04d6486cb7ee</x:t>
-  </x:si>
-  <x:si>
-    <x:t>f20200042@pilani.bits-pilani.ac.in</x:t>
+    <x:t>612c457b82a6e7f8ae653d04</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MOHIT 20</x:t>
+  </x:si>
+  <x:si>
+    <x:t>f20180147@pilani.bits-pilani.ac.in</x:t>
   </x:si>
   <x:si>
     <x:t>Tue Sep 21 2021 16:30:00 GMT+0000 (Coordinated Universal Time)</x:t>
   </x:si>
   <x:si>
-    <x:t>612b72f2fdaa04d6486cb7f0</x:t>
-  </x:si>
-  <x:si>
-    <x:t>f20180041@pilani.bits-pilani.ac.in</x:t>
+    <x:t>612c458f82a6e7f8ae653d06</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MOHIT 11</x:t>
+  </x:si>
+  <x:si>
+    <x:t>f20191047@pilani.bits-pilani.ac.in</x:t>
   </x:si>
   <x:si>
     <x:t>Tue Sep 21 2021 16:30:00 GMT+0000 (Coordinated Universal Time)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>612b72fafdaa04d6486cb7f2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>f20190040@pilani.bits-pilani.ac.in</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tue Sep 21 2021 16:30:00 GMT+0000 (Coordinated Universal Time)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>612b7392d01c4e002d9b85e4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://lh3.googleusercontent.com/a-/AOh14GjEkCRdgPIW745KrN6wCdhRnqWpeZ4lhGHrwE7HbQ=s96-c</x:t>
-  </x:si>
-  <x:si>
-    <x:t>AKSHAT KUMAR</x:t>
-  </x:si>
-  <x:si>
-    <x:t>f20201976@pilani.bits-pilani.ac.in</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sun Aug 29 2021 17:14:52 GMT+0000 (Coordinated Universal Time)</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -681,10 +702,10 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E4" s="0" t="s">
         <x:v>18</x:v>
@@ -711,21 +732,21 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="M4" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:14">
       <x:c r="A5" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="E5" s="0" t="s">
         <x:v>18</x:v>
@@ -752,21 +773,21 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="M5" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:14">
       <x:c r="A6" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="E6" s="0" t="s">
         <x:v>18</x:v>
@@ -793,21 +814,21 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="M6" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:14">
       <x:c r="A7" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="E7" s="0" t="s">
         <x:v>18</x:v>
@@ -834,21 +855,21 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="M7" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:14">
       <x:c r="A8" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="E8" s="0" t="s">
         <x:v>18</x:v>
@@ -875,21 +896,21 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="M8" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>47</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:14">
       <x:c r="A9" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="E9" s="0" t="s">
         <x:v>18</x:v>
@@ -916,21 +937,21 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="M9" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>51</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:14">
       <x:c r="A10" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="E10" s="0" t="s">
         <x:v>18</x:v>
@@ -957,21 +978,21 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="M10" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>55</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:14">
       <x:c r="A11" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="E11" s="0" t="s">
         <x:v>18</x:v>
@@ -998,27 +1019,27 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="M11" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>59</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:14">
       <x:c r="A12" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="E12" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="F12" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="G12" s="0" t="s">
         <x:v>20</x:v>
@@ -1026,6 +1047,12 @@
       <x:c r="H12" s="0" t="b">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="I12" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="J12" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
       <x:c r="K12" s="0" t="b">
         <x:v>1</x:v>
       </x:c>
@@ -1033,7 +1060,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="M12" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>63</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>